<commit_message>
Update arduino pinout with built-in LED on D13
</commit_message>
<xml_diff>
--- a/hardware/arduino_pinout.xlsx
+++ b/hardware/arduino_pinout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="83">
   <si>
     <t>Tumbller Self-Balancing Car IO Pin Connection Table</t>
   </si>
@@ -91,7 +91,7 @@
     <t>RGB</t>
   </si>
   <si>
-    <t>LEDS</t>
+    <t>LED_RGB</t>
   </si>
   <si>
     <t>RGB LED control pin</t>
@@ -190,61 +190,67 @@
     <t>D13</t>
   </si>
   <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LED_BUILTIN</t>
+  </si>
+  <si>
+    <t>Built-in nano LED pin</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>328P Receiver pin/Left IR Receiver pin</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>328P Receiver pin/Right IR Receiver pin</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>VOL</t>
+  </si>
+  <si>
+    <t>ANALOG</t>
+  </si>
+  <si>
+    <t>BATTERY</t>
+  </si>
+  <si>
+    <t>Battery voltage detection pin</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>ECHO</t>
+  </si>
+  <si>
+    <t>Ultrasonic echo pin</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>OPEN_DRAIN</t>
+  </si>
+  <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Unused pin</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>328P Receiver pin/Left IR Receiver pin</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>328P Receiver pin/Right IR Receiver pin</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>VOL</t>
-  </si>
-  <si>
-    <t>ANALOG</t>
-  </si>
-  <si>
-    <t>BATTERY</t>
-  </si>
-  <si>
-    <t>Battery voltage detection pin</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>ECHO</t>
-  </si>
-  <si>
-    <t>Ultrasonic echo pin</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>I2C</t>
-  </si>
-  <si>
-    <t>OPEN_DRAIN</t>
   </si>
   <si>
     <t>IMU</t>
@@ -264,7 +270,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,19 +287,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
     </font>
@@ -443,14 +443,14 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,14 +760,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="13" width="19.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="15.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="16.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="14.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="48.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="12" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="15.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="16.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="14.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="48.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="13" width="16.433571428571426" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="13" width="13.147857142857141" customWidth="1" bestFit="1"/>
@@ -1204,19 +1204,19 @@
         <v>58</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
@@ -1227,10 +1227,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21">
       <c r="A17" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>20</v>
@@ -1239,27 +1239,27 @@
         <v>11</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="11" t="s">
-        <v>62</v>
+      <c r="G17" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="H17" s="2"/>
       <c r="I17" s="3"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="12"/>
+      <c r="M17" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="21">
       <c r="A18" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>20</v>
@@ -1268,30 +1268,30 @@
         <v>11</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="11" t="s">
-        <v>64</v>
+      <c r="G18" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="12"/>
+      <c r="M18" s="11"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21">
       <c r="A19" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>11</v>
@@ -1300,10 +1300,10 @@
         <v>12</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
@@ -1314,10 +1314,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="21">
       <c r="A20" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>20</v>
@@ -1332,7 +1332,7 @@
         <v>52</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
@@ -1343,25 +1343,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="21">
       <c r="A21" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
@@ -1372,22 +1372,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="21.75">
       <c r="A22" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="2"/>

</xml_diff>